<commit_message>
fixed carwash sql file with new data
</commit_message>
<xml_diff>
--- a/Carwash Project/Carwash Mapeo.xlsx
+++ b/Carwash Project/Carwash Mapeo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\databases-1\Carwash Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7E9955-90FC-47B6-B8FB-08118D3201B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9B1ADF-82E3-4068-9016-B7C11C56CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F604237-8166-4D78-AF33-CFCAF7076FF4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
   <si>
     <t>PERSONA</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Pérez</t>
   </si>
   <si>
-    <t>Av. Siempre Viva 123</t>
-  </si>
-  <si>
     <t>555-1234</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Gómez</t>
   </si>
   <si>
-    <t>Calle Falsa 456</t>
-  </si>
-  <si>
     <t>555-5678</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
     <t>Mediano</t>
   </si>
   <si>
-    <t>Auto</t>
-  </si>
-  <si>
     <t>Honda</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
     <t>Pequeño</t>
   </si>
   <si>
-    <t>Moto</t>
-  </si>
-  <si>
     <t>Sombrero</t>
   </si>
   <si>
@@ -315,6 +303,21 @@
   </si>
   <si>
     <t>j.perezl@gmail.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Calle Bolivar 456</t>
+  </si>
+  <si>
+    <t>Av. Brasil 432</t>
+  </si>
+  <si>
+    <t>EmpleadoCI</t>
   </si>
 </sst>
 </file>
@@ -440,45 +443,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -814,17 +809,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB1C885-2198-4FCB-9455-7C76938D152E}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="4.140625" customWidth="1"/>
@@ -871,24 +867,24 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="10"/>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="8"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -901,95 +897,95 @@
         <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="25"/>
+      <c r="F4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="L4" s="1">
         <v>7679493</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="18">
         <v>44941</v>
       </c>
-      <c r="N4" s="11"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>7328931</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="7"/>
+      <c r="I5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="10"/>
       <c r="L5" s="1">
         <v>7328931</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="18">
         <v>44977</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7436482</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="7"/>
+      <c r="I6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="10"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -997,14 +993,14 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1056,13 +1052,13 @@
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="19"/>
+      <c r="F12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="17"/>
       <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1087,125 +1083,125 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>59</v>
+      <c r="E13" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F13" s="1">
         <v>7679493</v>
       </c>
-      <c r="H13" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="5">
+      <c r="H13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="4">
         <v>4</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M13" s="5">
+        <v>81</v>
+      </c>
+      <c r="M13" s="4">
         <v>600</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P13" s="14">
+        <v>79</v>
+      </c>
+      <c r="P13" s="4">
         <v>1</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F14" s="1">
         <v>7328931</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="5">
+      <c r="H14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="4">
         <v>4</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="5"/>
+      <c r="M14" s="4"/>
       <c r="O14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P14" s="14">
+        <v>80</v>
+      </c>
+      <c r="P14" s="4">
         <v>2</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F15" s="1">
         <v>7679493</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="5"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="4"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="4"/>
       <c r="O15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P15" s="14">
+        <v>81</v>
+      </c>
+      <c r="P15" s="4">
         <v>3</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1215,17 +1211,17 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="4"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="5"/>
+      <c r="M16" s="4"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="5"/>
+      <c r="P16" s="4"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1237,7 +1233,7 @@
       </c>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1255,17 +1251,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="10"/>
       <c r="F21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1275,152 +1271,149 @@
       <c r="H21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="21"/>
+      <c r="J21" s="9"/>
       <c r="K21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="M21" s="22"/>
+      <c r="L21" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M21" s="15"/>
       <c r="O21" s="3" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>7436482</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="9">
+        <v>52</v>
+      </c>
+      <c r="C22" s="21">
         <v>45087</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="F22" s="5">
+      <c r="D22" s="21"/>
+      <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="5">
         <v>45444</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="7">
         <v>0.375</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="J22" s="21"/>
+      <c r="I22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="9"/>
       <c r="K22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M22" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="10"/>
       <c r="O22" s="1">
         <v>7436482</v>
       </c>
-      <c r="P22" s="5">
+      <c r="P22" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>7328931</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="9">
+        <v>53</v>
+      </c>
+      <c r="C23" s="21">
         <v>44788</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="F23" s="5">
+      <c r="D23" s="21"/>
+      <c r="F23" s="4">
         <v>2</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="5">
         <v>45445</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I23" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="J23" s="21"/>
+      <c r="I23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="9"/>
       <c r="K23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="10"/>
       <c r="O23" s="1">
         <v>7436482</v>
       </c>
-      <c r="P23" s="5">
+      <c r="P23" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="F24" s="5">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="F24" s="4">
         <v>3</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="5">
         <v>45446</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="I24" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="J24" s="21"/>
+      <c r="I24" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J24" s="9"/>
       <c r="K24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M24" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="10"/>
       <c r="O24" s="1">
         <v>7436482</v>
       </c>
-      <c r="P24" s="5">
+      <c r="P24" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="F25" s="5"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="5"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S27" s="23"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P25" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1422,7 @@
       </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
@@ -1440,17 +1433,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1460,99 +1453,134 @@
       <c r="H30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
+        <v>2</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="4">
+        <v>2</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1</v>
-      </c>
-      <c r="H31" s="5">
-        <v>2</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" s="5">
-        <v>2</v>
-      </c>
-      <c r="H32" s="5">
-        <v>2</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="D33" s="9"/>
+      <c r="E33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="4">
         <v>3</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="H33" s="4">
         <v>3</v>
       </c>
-      <c r="H33" s="5">
-        <v>3</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="J33" s="7"/>
+      <c r="I33" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="1"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
@@ -1562,42 +1590,7 @@
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{A7EE819F-767A-4812-8045-29FE08A20DCE}"/>

</xml_diff>

<commit_message>
new data, need to be fixed
</commit_message>
<xml_diff>
--- a/Carwash Project/Carwash Mapeo.xlsx
+++ b/Carwash Project/Carwash Mapeo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\databases-1\Carwash Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ACB578-407D-49A7-8337-A6DD4CF05432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21112B65-1761-4EC6-AE85-89CF88B0DB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{0F604237-8166-4D78-AF33-CFCAF7076FF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F604237-8166-4D78-AF33-CFCAF7076FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="131">
   <si>
     <t>PERSONA</t>
   </si>
@@ -185,12 +185,6 @@
     <t>5424BOL</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -248,9 +242,6 @@
     <t>Alarcón</t>
   </si>
   <si>
-    <t xml:space="preserve">Lucas </t>
-  </si>
-  <si>
     <t>Lino</t>
   </si>
   <si>
@@ -359,9 +350,6 @@
     <t>3456ANA</t>
   </si>
   <si>
-    <t xml:space="preserve">Suzuki </t>
-  </si>
-  <si>
     <t>Vitara</t>
   </si>
   <si>
@@ -429,12 +417,28 @@
   </si>
   <si>
     <t>Lavado y desengrasado</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>En Proceso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;Bs&quot;#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="&quot;Bs&quot;#,##0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,7 +504,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -558,91 +562,128 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB1C885-2198-4FCB-9455-7C76938D152E}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,241 +1078,241 @@
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>7436482</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" s="4">
         <v>69156782</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="7"/>
+      <c r="F4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>7328931</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="4">
         <v>66843426</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="7"/>
+      <c r="F5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4837241</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E6" s="4">
         <v>67487322</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="6"/>
+      <c r="F6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1562892</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E7" s="4">
         <v>64924121</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="6"/>
+      <c r="F7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7772831</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4">
         <v>72893411</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="6"/>
+      <c r="F8" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7392432</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E9" s="4">
         <v>77138283</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
+      <c r="F9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>4563234</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E10" s="4">
         <v>77732151</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="6"/>
+      <c r="F10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7323912</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11" s="4">
         <v>67301991</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="6"/>
+      <c r="F11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>7679493</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="4">
         <v>77543643</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="7"/>
+      <c r="F12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="26"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1320,16 +1361,16 @@
       <c r="D17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="15" t="s">
+      <c r="F17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="16"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="4" t="s">
         <v>19</v>
       </c>
@@ -1348,299 +1389,300 @@
       <c r="Q17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R17" s="7" t="s">
+      <c r="R17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="S17" s="7"/>
+      <c r="S17" s="12"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>51</v>
+      <c r="E18" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F18" s="4">
         <v>1562892</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="17">
+      <c r="I18" s="37"/>
+      <c r="J18" s="7">
         <v>4</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="38">
         <v>200</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="17">
+      <c r="P18" s="7">
         <v>1</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="S18" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="S18" s="12"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>51</v>
+      <c r="E19" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F19" s="4">
         <v>7328931</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="17">
+      <c r="I19" s="37"/>
+      <c r="J19" s="7">
         <v>2</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="M19" s="17">
+      <c r="L19" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="38">
         <v>250</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19" s="7">
         <v>2</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="S19" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="S19" s="12"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>52</v>
+      <c r="E20" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="F20" s="4">
         <v>4563234</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="17">
+      <c r="H20" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="37"/>
+      <c r="J20" s="7">
         <v>2</v>
       </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="17"/>
+      <c r="M20" s="7"/>
       <c r="O20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="P20" s="17">
+        <v>54</v>
+      </c>
+      <c r="P20" s="7">
         <v>3</v>
       </c>
       <c r="Q20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="R20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="S20" s="7"/>
+      <c r="R20" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S20" s="12"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>51</v>
+      <c r="E21" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F21" s="4">
         <v>7679493</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="17">
+      <c r="H21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="37"/>
+      <c r="J21" s="7">
         <v>4</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="17"/>
+      <c r="M21" s="7"/>
       <c r="O21" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P21" s="17">
+        <v>103</v>
+      </c>
+      <c r="P21" s="7">
         <v>4</v>
       </c>
       <c r="Q21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="R21" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="R21" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="S21" s="7"/>
+      <c r="S21" s="12"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F22" s="4">
         <v>7323912</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="17">
+      <c r="H22" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="37"/>
+      <c r="J22" s="7">
         <v>4</v>
       </c>
-      <c r="M22" s="18"/>
+      <c r="M22" s="8"/>
       <c r="O22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P22" s="17">
+        <v>53</v>
+      </c>
+      <c r="P22" s="7">
         <v>5</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="S22" s="7"/>
+        <v>122</v>
+      </c>
+      <c r="R22" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="S22" s="12"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="E23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="33">
         <v>4837241</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="17">
+      <c r="H23" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="37"/>
+      <c r="J23" s="7">
         <v>4</v>
       </c>
-      <c r="M23" s="18"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>51</v>
+      <c r="E24" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F24" s="4">
         <v>7772831</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="M24" s="18"/>
+      <c r="J24" s="8"/>
+      <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F25" s="4">
         <v>7436482</v>
       </c>
-      <c r="J25" s="18"/>
-      <c r="M25" s="18"/>
+      <c r="J25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="11"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1661,10 +1703,10 @@
       <c r="D29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L29" s="19"/>
+      <c r="L29" s="24"/>
       <c r="N29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1685,23 +1727,23 @@
       <c r="E30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="4" t="s">
+      <c r="H30" s="12"/>
+      <c r="I30" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="20" t="s">
+      <c r="J30" s="30"/>
+      <c r="K30" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="L30" s="20"/>
+      <c r="L30" s="25"/>
       <c r="N30" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>27</v>
@@ -1714,31 +1756,31 @@
       <c r="B31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="7">
         <v>1</v>
       </c>
-      <c r="E31" s="21">
-        <v>45469</v>
-      </c>
-      <c r="F31" s="22">
+      <c r="E31" s="9">
+        <v>45463</v>
+      </c>
+      <c r="F31" s="10">
         <v>0.375</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7">
+      <c r="G31" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13">
         <v>110</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7" t="s">
+      <c r="J31" s="13"/>
+      <c r="K31" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="L31" s="7"/>
+      <c r="L31" s="13"/>
       <c r="N31" s="4">
         <v>7436482</v>
       </c>
-      <c r="O31" s="17">
+      <c r="O31" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1747,36 +1789,36 @@
         <v>7328931</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="17">
+        <v>105</v>
+      </c>
+      <c r="D32" s="7">
         <v>2</v>
       </c>
-      <c r="E32" s="21">
-        <v>45469</v>
-      </c>
-      <c r="F32" s="22">
+      <c r="E32" s="9">
+        <v>45463</v>
+      </c>
+      <c r="F32" s="10">
         <v>0.4375</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7">
+      <c r="G32" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="13">
         <v>150</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7" t="s">
+      <c r="J32" s="13"/>
+      <c r="K32" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="L32" s="7"/>
+      <c r="L32" s="13"/>
       <c r="N32" s="4">
         <v>7328931</v>
       </c>
-      <c r="O32" s="17">
+      <c r="O32" s="7">
         <v>2</v>
       </c>
-      <c r="Q32" s="23"/>
+      <c r="Q32" s="11"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
@@ -1785,31 +1827,31 @@
       <c r="B33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="7">
         <v>3</v>
       </c>
-      <c r="E33" s="21">
-        <v>45470</v>
-      </c>
-      <c r="F33" s="22">
+      <c r="E33" s="9">
+        <v>45464</v>
+      </c>
+      <c r="F33" s="10">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7">
+      <c r="G33" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13">
         <v>100</v>
       </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L33" s="7"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="13"/>
       <c r="N33" s="4">
         <v>4837241</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1820,31 +1862,31 @@
       <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="7">
         <v>4</v>
       </c>
-      <c r="E34" s="21">
-        <v>45471</v>
-      </c>
-      <c r="F34" s="22">
+      <c r="E34" s="9">
+        <v>45465</v>
+      </c>
+      <c r="F34" s="10">
         <v>0.5</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7">
+      <c r="G34" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13">
         <v>90</v>
       </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="L34" s="7"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L34" s="13"/>
       <c r="N34" s="4">
         <v>1562892</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1853,239 +1895,567 @@
         <v>7772831</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="18"/>
+        <v>106</v>
+      </c>
+      <c r="D35" s="7">
+        <v>5</v>
+      </c>
+      <c r="E35" s="9">
+        <v>45466</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="13">
+        <v>45</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" s="12"/>
       <c r="N35" s="4">
         <v>7772831</v>
       </c>
-      <c r="O35" s="17">
+      <c r="O35" s="7">
         <v>5</v>
       </c>
     </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="D36" s="7">
+        <v>6</v>
+      </c>
+      <c r="E36" s="9">
+        <v>45467</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13">
+        <v>140</v>
+      </c>
+      <c r="J36" s="13"/>
+      <c r="K36" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L36" s="12"/>
+      <c r="N36" s="4">
+        <v>7436482</v>
+      </c>
+      <c r="O36" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="D37" s="7">
+        <v>7</v>
+      </c>
+      <c r="E37" s="9">
+        <v>45468</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="13">
+        <v>100</v>
+      </c>
+      <c r="J37" s="13"/>
+      <c r="K37" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="12"/>
+      <c r="N37" s="4">
+        <v>7328931</v>
+      </c>
+      <c r="O37" s="7">
+        <v>7</v>
+      </c>
+    </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="D38" s="7">
+        <v>8</v>
+      </c>
+      <c r="E38" s="9">
+        <v>45469</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="13">
+        <v>180</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" s="12"/>
+      <c r="N38" s="4">
+        <v>4837241</v>
+      </c>
+      <c r="O38" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="D39" s="7">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9">
+        <v>45470</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="13">
+        <v>70</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" s="12"/>
+      <c r="N39" s="4">
+        <v>1562892</v>
+      </c>
+      <c r="O39" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D40" s="7">
+        <v>10</v>
+      </c>
+      <c r="E40" s="9">
+        <v>45470</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13">
+        <v>170</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" s="12"/>
+      <c r="N40" s="4">
+        <v>7772831</v>
+      </c>
+      <c r="O40" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E41" s="35"/>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C45" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="4" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I45" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+      <c r="J45" s="32"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>1</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B46" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="39">
+        <v>40</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7">
+        <v>1</v>
+      </c>
+      <c r="I46" s="22">
+        <v>30</v>
+      </c>
+      <c r="J46" s="23"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>2</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="39">
+        <v>100</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7">
+        <v>3</v>
+      </c>
+      <c r="I47" s="22">
+        <v>80</v>
+      </c>
+      <c r="J47" s="23"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>3</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C48" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="4">
+      <c r="D48" s="15"/>
+      <c r="E48" s="39">
+        <v>70</v>
+      </c>
+      <c r="G48" s="7">
+        <v>2</v>
+      </c>
+      <c r="H48" s="7">
+        <v>2</v>
+      </c>
+      <c r="I48" s="22">
+        <v>100</v>
+      </c>
+      <c r="J48" s="23"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>4</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="39">
+        <v>50</v>
+      </c>
+      <c r="G49" s="7">
+        <v>2</v>
+      </c>
+      <c r="H49" s="7">
+        <v>3</v>
+      </c>
+      <c r="I49" s="22">
+        <v>50</v>
+      </c>
+      <c r="J49" s="23"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>5</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="39">
+        <v>100</v>
+      </c>
+      <c r="G50" s="7">
+        <v>3</v>
+      </c>
+      <c r="H50" s="7">
+        <v>5</v>
+      </c>
+      <c r="I50" s="22">
+        <v>100</v>
+      </c>
+      <c r="J50" s="23"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G51" s="7">
+        <v>4</v>
+      </c>
+      <c r="H51" s="7">
+        <v>1</v>
+      </c>
+      <c r="I51" s="22">
         <v>40</v>
       </c>
-      <c r="G41" s="17">
+      <c r="J51" s="23"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G52" s="7">
+        <v>4</v>
+      </c>
+      <c r="H52" s="7">
+        <v>4</v>
+      </c>
+      <c r="I52" s="22">
+        <v>50</v>
+      </c>
+      <c r="J52" s="23"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G53" s="7">
+        <v>5</v>
+      </c>
+      <c r="H53" s="7">
+        <v>4</v>
+      </c>
+      <c r="I53" s="22">
+        <v>45</v>
+      </c>
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G54" s="7">
+        <v>6</v>
+      </c>
+      <c r="H54" s="7">
         <v>1</v>
       </c>
-      <c r="H41" s="17">
+      <c r="I54" s="22">
+        <v>40</v>
+      </c>
+      <c r="J54" s="23"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G55" s="7">
+        <v>6</v>
+      </c>
+      <c r="H55" s="7">
+        <v>5</v>
+      </c>
+      <c r="I55" s="22">
+        <v>100</v>
+      </c>
+      <c r="J55" s="23"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G56" s="7">
+        <v>7</v>
+      </c>
+      <c r="H56" s="7">
+        <v>2</v>
+      </c>
+      <c r="I56" s="22">
+        <v>50</v>
+      </c>
+      <c r="J56" s="23"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G57" s="7">
+        <v>7</v>
+      </c>
+      <c r="H57" s="7">
+        <v>3</v>
+      </c>
+      <c r="I57" s="22">
+        <v>50</v>
+      </c>
+      <c r="J57" s="23"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G58" s="7">
+        <v>8</v>
+      </c>
+      <c r="H58" s="7">
+        <v>4</v>
+      </c>
+      <c r="I58" s="22">
+        <v>50</v>
+      </c>
+      <c r="J58" s="23"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G59" s="7">
+        <v>8</v>
+      </c>
+      <c r="H59" s="7">
         <v>1</v>
       </c>
-      <c r="I41" s="5">
-        <v>30</v>
-      </c>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="I59" s="22">
+        <v>40</v>
+      </c>
+      <c r="J59" s="23"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G60" s="7">
+        <v>9</v>
+      </c>
+      <c r="H60" s="7">
+        <v>3</v>
+      </c>
+      <c r="I60" s="22">
+        <v>70</v>
+      </c>
+      <c r="J60" s="23"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G61" s="7">
+        <v>10</v>
+      </c>
+      <c r="H61" s="7">
         <v>2</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="4">
+      <c r="I61" s="22">
         <v>100</v>
       </c>
-      <c r="G42" s="17">
+      <c r="J61" s="23"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G62" s="7">
+        <v>10</v>
+      </c>
+      <c r="H62" s="7">
         <v>1</v>
       </c>
-      <c r="H42" s="17">
-        <v>3</v>
-      </c>
-      <c r="I42" s="5">
-        <v>80</v>
-      </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
-        <v>3</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="4">
+      <c r="I62" s="22">
         <v>70</v>
       </c>
-      <c r="G43" s="17">
-        <v>2</v>
-      </c>
-      <c r="H43" s="17">
-        <v>2</v>
-      </c>
-      <c r="I43" s="5">
-        <v>100</v>
-      </c>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
-        <v>4</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="4">
-        <v>50</v>
-      </c>
-      <c r="G44" s="17">
-        <v>2</v>
-      </c>
-      <c r="H44" s="17">
-        <v>3</v>
-      </c>
-      <c r="I44" s="5">
-        <v>50</v>
-      </c>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
-        <v>5</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="4">
-        <v>100</v>
-      </c>
-      <c r="G45" s="17">
-        <v>3</v>
-      </c>
-      <c r="H45" s="17">
-        <v>5</v>
-      </c>
-      <c r="I45" s="5">
-        <v>100</v>
-      </c>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G46" s="17">
-        <v>4</v>
-      </c>
-      <c r="H46" s="17">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5">
-        <v>40</v>
-      </c>
-      <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G47" s="17">
-        <v>4</v>
-      </c>
-      <c r="H47" s="17">
-        <v>4</v>
-      </c>
-      <c r="I47" s="5">
-        <v>50</v>
-      </c>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G48" s="17">
-        <v>5</v>
-      </c>
-      <c r="H48" s="17">
-        <v>4</v>
-      </c>
-      <c r="I48" s="5">
-        <v>45</v>
-      </c>
-      <c r="J48" s="6"/>
+      <c r="J62" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="91">
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K40:L40"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I53:J53"/>
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="R18:S18"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="R20:S20"/>
     <mergeCell ref="R21:S21"/>
     <mergeCell ref="R22:S22"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K35:L35"/>
     <mergeCell ref="C45:D45"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
@@ -2094,16 +2464,19 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F5:G5"/>
@@ -2114,25 +2487,8 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>